<commit_message>
new spinner with compass
</commit_message>
<xml_diff>
--- a/data/download.xlsx
+++ b/data/download.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>Fecha</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>PVPC</t>
+  </si>
+  <si>
+    <t>Verano</t>
   </si>
   <si>
     <t>España</t>
@@ -55,9 +58,6 @@
   </si>
   <si>
     <t>Reino Unido</t>
-  </si>
-  <si>
-    <t>Verano</t>
   </si>
   <si>
     <t>Península</t>
@@ -434,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -455,6 +455,414 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>84.8</v>
+      </c>
+      <c r="E2">
+        <v>133.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>76.5</v>
+      </c>
+      <c r="E3">
+        <v>125.51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>70.12</v>
+      </c>
+      <c r="E4">
+        <v>121.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>120.63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
+      <c r="E6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>54.08</v>
+      </c>
+      <c r="E7">
+        <v>102.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>63.38</v>
+      </c>
+      <c r="E8">
+        <v>110.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>84.34</v>
+      </c>
+      <c r="E9">
+        <v>130.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>83.93000000000001</v>
+      </c>
+      <c r="E10">
+        <v>158.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>82.27</v>
+      </c>
+      <c r="E11">
+        <v>158.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>55</v>
+      </c>
+      <c r="E12">
+        <v>176.29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>119.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>3.32</v>
+      </c>
+      <c r="E14">
+        <v>115.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>3.32</v>
+      </c>
+      <c r="E15">
+        <v>115.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1.51</v>
+      </c>
+      <c r="E16">
+        <v>63.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>0.44</v>
+      </c>
+      <c r="E17">
+        <v>63.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>0.44</v>
+      </c>
+      <c r="E18">
+        <v>63.46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>3.32</v>
+      </c>
+      <c r="E19">
+        <v>67.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>49.97</v>
+      </c>
+      <c r="E20">
+        <v>171.87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>82.27</v>
+      </c>
+      <c r="E21">
+        <v>205.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>82.27</v>
+      </c>
+      <c r="E22">
+        <v>201.44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>72.59</v>
+      </c>
+      <c r="E23">
+        <v>192.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>71.08</v>
+      </c>
+      <c r="E24">
+        <v>144.43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>68.06</v>
+      </c>
+      <c r="E25">
+        <v>143.89</v>
       </c>
     </row>
   </sheetData>
@@ -481,28 +889,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -513,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>84.8</v>
@@ -533,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>76.5</v>
@@ -553,7 +961,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>70.12</v>
@@ -573,7 +981,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>70</v>
@@ -593,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>60</v>
@@ -613,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>54.08</v>
@@ -633,7 +1041,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>63.38</v>
@@ -653,7 +1061,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>84.34</v>
@@ -673,7 +1081,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>83.93000000000001</v>
@@ -693,7 +1101,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>82.27</v>
@@ -713,7 +1121,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>55</v>
@@ -733,7 +1141,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -753,7 +1161,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>3.32</v>
@@ -773,7 +1181,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>3.32</v>
@@ -793,7 +1201,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>1.51</v>
@@ -813,7 +1221,7 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>0.44</v>
@@ -833,7 +1241,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D18">
         <v>0.44</v>
@@ -853,7 +1261,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>3.32</v>
@@ -873,7 +1281,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>49.97</v>
@@ -893,7 +1301,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>82.27</v>
@@ -913,7 +1321,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>82.27</v>
@@ -933,7 +1341,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>72.59</v>
@@ -953,7 +1361,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>71.08</v>
@@ -973,7 +1381,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>68.06</v>
@@ -992,7 +1400,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1024,6 +1432,630 @@
         <v>18</v>
       </c>
     </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>133.7</v>
+      </c>
+      <c r="E2">
+        <v>133.7</v>
+      </c>
+      <c r="F2">
+        <v>133.7</v>
+      </c>
+      <c r="G2">
+        <v>133.7</v>
+      </c>
+      <c r="H2">
+        <v>133.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>125.51</v>
+      </c>
+      <c r="E3">
+        <v>125.51</v>
+      </c>
+      <c r="F3">
+        <v>125.51</v>
+      </c>
+      <c r="G3">
+        <v>125.51</v>
+      </c>
+      <c r="H3">
+        <v>125.51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>121.32</v>
+      </c>
+      <c r="E4">
+        <v>121.32</v>
+      </c>
+      <c r="F4">
+        <v>121.32</v>
+      </c>
+      <c r="G4">
+        <v>121.32</v>
+      </c>
+      <c r="H4">
+        <v>121.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>120.63</v>
+      </c>
+      <c r="E5">
+        <v>120.63</v>
+      </c>
+      <c r="F5">
+        <v>120.63</v>
+      </c>
+      <c r="G5">
+        <v>120.63</v>
+      </c>
+      <c r="H5">
+        <v>120.63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>110</v>
+      </c>
+      <c r="F6">
+        <v>110</v>
+      </c>
+      <c r="G6">
+        <v>110</v>
+      </c>
+      <c r="H6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>102.1</v>
+      </c>
+      <c r="E7">
+        <v>102.1</v>
+      </c>
+      <c r="F7">
+        <v>102.1</v>
+      </c>
+      <c r="G7">
+        <v>102.1</v>
+      </c>
+      <c r="H7">
+        <v>102.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>110.59</v>
+      </c>
+      <c r="E8">
+        <v>110.59</v>
+      </c>
+      <c r="F8">
+        <v>110.59</v>
+      </c>
+      <c r="G8">
+        <v>110.59</v>
+      </c>
+      <c r="H8">
+        <v>110.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>130.15</v>
+      </c>
+      <c r="E9">
+        <v>130.15</v>
+      </c>
+      <c r="F9">
+        <v>130.15</v>
+      </c>
+      <c r="G9">
+        <v>130.15</v>
+      </c>
+      <c r="H9">
+        <v>130.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>158.28</v>
+      </c>
+      <c r="E10">
+        <v>158.28</v>
+      </c>
+      <c r="F10">
+        <v>158.28</v>
+      </c>
+      <c r="G10">
+        <v>158.28</v>
+      </c>
+      <c r="H10">
+        <v>158.28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>158.11</v>
+      </c>
+      <c r="E11">
+        <v>158.11</v>
+      </c>
+      <c r="F11">
+        <v>158.11</v>
+      </c>
+      <c r="G11">
+        <v>158.11</v>
+      </c>
+      <c r="H11">
+        <v>158.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>176.29</v>
+      </c>
+      <c r="E12">
+        <v>176.29</v>
+      </c>
+      <c r="F12">
+        <v>176.29</v>
+      </c>
+      <c r="G12">
+        <v>126.03</v>
+      </c>
+      <c r="H12">
+        <v>126.03</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>119.92</v>
+      </c>
+      <c r="E13">
+        <v>119.92</v>
+      </c>
+      <c r="F13">
+        <v>119.92</v>
+      </c>
+      <c r="G13">
+        <v>119.92</v>
+      </c>
+      <c r="H13">
+        <v>119.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>115.16</v>
+      </c>
+      <c r="E14">
+        <v>115.16</v>
+      </c>
+      <c r="F14">
+        <v>115.16</v>
+      </c>
+      <c r="G14">
+        <v>115.16</v>
+      </c>
+      <c r="H14">
+        <v>115.16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>115.03</v>
+      </c>
+      <c r="E15">
+        <v>115.03</v>
+      </c>
+      <c r="F15">
+        <v>115.03</v>
+      </c>
+      <c r="G15">
+        <v>115.03</v>
+      </c>
+      <c r="H15">
+        <v>115.03</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>63.86</v>
+      </c>
+      <c r="E16">
+        <v>63.86</v>
+      </c>
+      <c r="F16">
+        <v>63.86</v>
+      </c>
+      <c r="G16">
+        <v>113.91</v>
+      </c>
+      <c r="H16">
+        <v>113.91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>63.03</v>
+      </c>
+      <c r="E17">
+        <v>63.03</v>
+      </c>
+      <c r="F17">
+        <v>63.03</v>
+      </c>
+      <c r="G17">
+        <v>63.03</v>
+      </c>
+      <c r="H17">
+        <v>63.03</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>63.46</v>
+      </c>
+      <c r="E18">
+        <v>63.46</v>
+      </c>
+      <c r="F18">
+        <v>63.46</v>
+      </c>
+      <c r="G18">
+        <v>63.46</v>
+      </c>
+      <c r="H18">
+        <v>63.46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>67.33</v>
+      </c>
+      <c r="E19">
+        <v>67.33</v>
+      </c>
+      <c r="F19">
+        <v>67.33</v>
+      </c>
+      <c r="G19">
+        <v>67.33</v>
+      </c>
+      <c r="H19">
+        <v>67.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>171.87</v>
+      </c>
+      <c r="E20">
+        <v>171.87</v>
+      </c>
+      <c r="F20">
+        <v>171.87</v>
+      </c>
+      <c r="G20">
+        <v>121.62</v>
+      </c>
+      <c r="H20">
+        <v>121.62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>205.3</v>
+      </c>
+      <c r="E21">
+        <v>205.3</v>
+      </c>
+      <c r="F21">
+        <v>205.3</v>
+      </c>
+      <c r="G21">
+        <v>205.3</v>
+      </c>
+      <c r="H21">
+        <v>205.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>201.44</v>
+      </c>
+      <c r="E22">
+        <v>201.44</v>
+      </c>
+      <c r="F22">
+        <v>201.44</v>
+      </c>
+      <c r="G22">
+        <v>201.44</v>
+      </c>
+      <c r="H22">
+        <v>201.44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>192.01</v>
+      </c>
+      <c r="E23">
+        <v>192.01</v>
+      </c>
+      <c r="F23">
+        <v>192.01</v>
+      </c>
+      <c r="G23">
+        <v>192.01</v>
+      </c>
+      <c r="H23">
+        <v>192.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>144.43</v>
+      </c>
+      <c r="E24">
+        <v>144.43</v>
+      </c>
+      <c r="F24">
+        <v>144.43</v>
+      </c>
+      <c r="G24">
+        <v>194.87</v>
+      </c>
+      <c r="H24">
+        <v>194.87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="2">
+        <v>45582</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>143.89</v>
+      </c>
+      <c r="E25">
+        <v>143.89</v>
+      </c>
+      <c r="F25">
+        <v>143.89</v>
+      </c>
+      <c r="G25">
+        <v>143.89</v>
+      </c>
+      <c r="H25">
+        <v>143.89</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>